<commit_message>
More tests on ATR-72 and A320. New feature: possibility to toogle the creation of CSV files for each plot.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/AIRBUS A-320/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/AIRBUS A-320/WEIGHTS/Weights.xlsx
@@ -346,7 +346,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>68885.4928957218</v>
+        <v>71762.6672440301</v>
       </c>
     </row>
     <row r="7">
@@ -357,7 +357,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>64645.49289572181</v>
+        <v>67522.6672440301</v>
       </c>
     </row>
     <row r="8">
@@ -368,7 +368,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>66818.92810885014</v>
+        <v>69609.7872267092</v>
       </c>
     </row>
     <row r="9">
@@ -390,7 +390,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>17638.63418025324</v>
+        <v>18075.552907740297</v>
       </c>
     </row>
     <row r="11">
@@ -401,7 +401,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>23212.319159666004</v>
+        <v>24181.838746069552</v>
       </c>
     </row>
     <row r="12">
@@ -423,7 +423,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>45673.17373605581</v>
+        <v>47580.82849796057</v>
       </c>
     </row>
     <row r="14">
@@ -434,7 +434,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>41433.17373605581</v>
+        <v>43340.82849796057</v>
       </c>
     </row>
     <row r="15">
@@ -445,7 +445,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>36133.17373605582</v>
+        <v>38040.828497960574</v>
       </c>
     </row>
     <row r="16">
@@ -456,7 +456,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="n">
-        <v>35559.202614714595</v>
+        <v>37452.47151617918</v>
       </c>
     </row>
     <row r="17">
@@ -467,7 +467,7 @@
         <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>34556.33009055581</v>
+        <v>36463.98485246058</v>
       </c>
     </row>
     <row r="18">
@@ -489,7 +489,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>344.4274758412121</v>
+        <v>358.81333628137986</v>
       </c>
     </row>
     <row r="20">
@@ -505,7 +505,7 @@
         <v>25</v>
       </c>
       <c r="C21" t="n">
-        <v>675535.91890583</v>
+        <v>703751.3607286676</v>
       </c>
     </row>
     <row r="22">
@@ -516,7 +516,7 @@
         <v>25</v>
       </c>
       <c r="C22" t="n">
-        <v>633955.72290583</v>
+        <v>662171.1647286676</v>
       </c>
     </row>
     <row r="23">
@@ -527,7 +527,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="n">
-        <v>655269.841338655</v>
+        <v>682638.8199068075</v>
       </c>
     </row>
     <row r="24">
@@ -549,7 +549,7 @@
         <v>25</v>
       </c>
       <c r="C25" t="n">
-        <v>172975.91188378038</v>
+        <v>177260.6209226913</v>
       </c>
     </row>
     <row r="26">
@@ -571,7 +571,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="n">
-        <v>447900.82921869156</v>
+        <v>466608.53178952483</v>
       </c>
     </row>
     <row r="28">
@@ -582,7 +582,7 @@
         <v>25</v>
       </c>
       <c r="C28" t="n">
-        <v>406320.63321869157</v>
+        <v>425028.33578952483</v>
       </c>
     </row>
     <row r="29">
@@ -593,7 +593,7 @@
         <v>25</v>
       </c>
       <c r="C29" t="n">
-        <v>354345.3882186917</v>
+        <v>373053.09078952495</v>
       </c>
     </row>
     <row r="30">
@@ -604,7 +604,7 @@
         <v>25</v>
       </c>
       <c r="C30" t="n">
-        <v>348716.6543215908</v>
+        <v>367283.2797941385</v>
       </c>
     </row>
     <row r="31">
@@ -615,7 +615,7 @@
         <v>25</v>
       </c>
       <c r="C31" t="n">
-        <v>338881.8344825491</v>
+        <v>357589.53705338243</v>
       </c>
     </row>
     <row r="32">
@@ -637,7 +637,7 @@
         <v>25</v>
       </c>
       <c r="C33" t="n">
-        <v>3377.6797059582213</v>
+        <v>3518.7568042437924</v>
       </c>
     </row>
   </sheetData>
@@ -713,9 +713,7 @@
       <c r="C6" t="n">
         <v>9743.0</v>
       </c>
-      <c r="D6" t="n">
-        <v>9.625879043600607</v>
-      </c>
+      <c r="D6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -725,11 +723,9 @@
         <v>43</v>
       </c>
       <c r="C7" t="n">
-        <v>7210.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-18.874824191279856</v>
-      </c>
+        <v>7304.0</v>
+      </c>
+      <c r="D7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -739,11 +735,9 @@
         <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>6703.0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-24.57946554149083</v>
-      </c>
+        <v>6842.0</v>
+      </c>
+      <c r="D8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -753,11 +747,9 @@
         <v>43</v>
       </c>
       <c r="C9" t="n">
-        <v>7121.0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-19.876230661040758</v>
-      </c>
+        <v>7403.0</v>
+      </c>
+      <c r="D9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -769,9 +761,7 @@
       <c r="C10" t="n">
         <v>7398.0</v>
       </c>
-      <c r="D10" t="n">
-        <v>-16.759493670886044</v>
-      </c>
+      <c r="D10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -783,9 +773,7 @@
       <c r="C11" t="n">
         <v>8693.0</v>
       </c>
-      <c r="D11" t="n">
-        <v>-2.188466947960579</v>
-      </c>
+      <c r="D11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -795,10 +783,10 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>7811.333333333332</v>
+        <v>8693.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-12.108766994842924</v>
+        <v>-2.1884669479605887</v>
       </c>
     </row>
   </sheetData>
@@ -897,10 +885,10 @@
         <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>6387.0</v>
+        <v>6380.0</v>
       </c>
       <c r="D8" t="n">
-        <v>7.797468354430412</v>
+        <v>7.679324894514801</v>
       </c>
     </row>
     <row r="9">
@@ -967,10 +955,10 @@
         <v>43</v>
       </c>
       <c r="C13" t="n">
-        <v>6694.0</v>
+        <v>6523.0</v>
       </c>
       <c r="D13" t="n">
-        <v>12.978902953586532</v>
+        <v>10.092827004219442</v>
       </c>
     </row>
     <row r="14">
@@ -981,10 +969,10 @@
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>5765.285714285714</v>
+        <v>5739.857142857143</v>
       </c>
       <c r="D14" t="n">
-        <v>-2.695599758890876</v>
+        <v>-3.124773960216978</v>
       </c>
     </row>
   </sheetData>
@@ -1097,10 +1085,10 @@
         <v>43</v>
       </c>
       <c r="C9" t="n">
-        <v>556.0</v>
+        <v>571.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-37.44022503516173</v>
+        <v>-35.75246132208156</v>
       </c>
     </row>
     <row r="10">
@@ -1111,10 +1099,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>485.0</v>
+        <v>623.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-45.428973277074526</v>
+        <v>-29.901547116736964</v>
       </c>
     </row>
   </sheetData>
@@ -1213,10 +1201,10 @@
         <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>427.0</v>
+        <v>421.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-51.95499296765119</v>
+        <v>-52.63009845288325</v>
       </c>
     </row>
     <row r="9">
@@ -1227,10 +1215,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>471.0</v>
+        <v>515.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-47.004219409282676</v>
+        <v>-42.05344585091419</v>
       </c>
     </row>
   </sheetData>
@@ -1283,10 +1271,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>893.3333333333333</v>
+        <v>1652.0</v>
       </c>
       <c r="D3" t="n">
-        <v>-66.49476480700108</v>
+        <v>-38.04031879981244</v>
       </c>
     </row>
     <row r="4">
@@ -1368,7 +1356,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>446.66666666666663</v>
+        <v>826.0</v>
       </c>
     </row>
     <row r="13">
@@ -1440,7 +1428,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>446.66666666666663</v>
+        <v>826.0</v>
       </c>
     </row>
     <row r="20">
@@ -1637,10 +1625,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>1918.0</v>
+        <v>1986.0</v>
       </c>
       <c r="D5" t="n">
-        <v>-19.07172995780588</v>
+        <v>-16.20253164556959</v>
       </c>
     </row>
     <row r="6">
@@ -1651,10 +1639,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>2755.0</v>
+        <v>2871.0</v>
       </c>
       <c r="D6" t="n">
-        <v>16.244725738396667</v>
+        <v>21.13924050632916</v>
       </c>
     </row>
     <row r="7">
@@ -1665,10 +1653,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>3183.0</v>
+        <v>3325.0</v>
       </c>
       <c r="D7" t="n">
-        <v>34.30379746835448</v>
+        <v>40.29535864978908</v>
       </c>
     </row>
     <row r="8">
@@ -1679,10 +1667,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>2791.0</v>
+        <v>2908.0</v>
       </c>
       <c r="D8" t="n">
-        <v>17.76371308016882</v>
+        <v>22.700421940928315</v>
       </c>
     </row>
     <row r="9">
@@ -1693,10 +1681,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>2661.75</v>
+        <v>2772.5</v>
       </c>
       <c r="D9" t="n">
-        <v>12.310126582278501</v>
+        <v>16.983122362869217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>